<commit_message>
F2 works for real finally
</commit_message>
<xml_diff>
--- a/Data/TabStats_Short_10C.xlsx
+++ b/Data/TabStats_Short_10C.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39451270-318F-45E0-9E15-E87E6BE62432}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A73C622-4E5C-44AF-804A-044FBCAE0066}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5235" yWindow="3945" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -444,8 +444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="J63" sqref="J63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>